<commit_message>
finishing caricoos and glos
</commit_message>
<xml_diff>
--- a/2024/data/processed/CARICOOS.xlsx
+++ b/2024/data/processed/CARICOOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathew.Biddle\Documents\GitProjects\ioos-asset-inventory\2024\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23999111-73E3-4B37-8F6D-7D925BE41FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F784BD58-6FD2-4F45-968A-A06D555886D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="198">
   <si>
     <t>Station ID</t>
   </si>
@@ -516,9 +516,6 @@
   </si>
   <si>
     <t>Yabucoa-El Negro, PR</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
   <si>
     <t>Mountain Top, USVI</t>
@@ -1534,7 +1531,7 @@
   <dimension ref="A1:U90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1572,13 +1569,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>193</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>3</v>
@@ -1587,19 +1584,19 @@
         <v>4</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>7</v>
@@ -1614,13 +1611,13 @@
         <v>10</v>
       </c>
       <c r="R1" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="S1" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="T1" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="U1" s="5"/>
     </row>
@@ -1677,7 +1674,7 @@
       </c>
       <c r="S2" s="12"/>
       <c r="T2" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -1733,7 +1730,7 @@
       </c>
       <c r="S3" s="12"/>
       <c r="T3" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -1789,7 +1786,7 @@
       </c>
       <c r="S4" s="12"/>
       <c r="T4" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -1845,7 +1842,7 @@
       </c>
       <c r="S5" s="12"/>
       <c r="T5" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -1903,7 +1900,7 @@
         <v>42</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -1961,7 +1958,7 @@
         <v>47</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="6" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2017,7 +2014,7 @@
       </c>
       <c r="S8" s="12"/>
       <c r="T8" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="6" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2073,7 +2070,7 @@
       </c>
       <c r="S9" s="12"/>
       <c r="T9" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -2128,7 +2125,7 @@
         <v>71</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="S10" s="18"/>
       <c r="T10" s="19" t="s">
@@ -2187,7 +2184,7 @@
         <v>82</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T11" s="9" t="s">
         <v>83</v>
@@ -2303,7 +2300,7 @@
         <v>94</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T13" s="9" t="s">
         <v>83</v>
@@ -2361,7 +2358,7 @@
         <v>82</v>
       </c>
       <c r="S14" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T14" s="9" t="s">
         <v>83</v>
@@ -2419,7 +2416,7 @@
         <v>102</v>
       </c>
       <c r="S15" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T15" s="9" t="s">
         <v>83</v>
@@ -3263,7 +3260,7 @@
         <v>89</v>
       </c>
       <c r="S30" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="T30" s="9" t="s">
         <v>83</v>
@@ -3326,14 +3323,10 @@
       </c>
     </row>
     <row r="32" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22" t="s">
         <v>159</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>160</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22">
@@ -3346,17 +3339,17 @@
         <v>77</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I32" s="22"/>
       <c r="J32" s="22" t="s">
         <v>45</v>
       </c>
       <c r="K32" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="L32" s="22" t="s">
         <v>162</v>
-      </c>
-      <c r="L32" s="22" t="s">
-        <v>163</v>
       </c>
       <c r="M32" s="23" t="s">
         <v>18</v>
@@ -3371,13 +3364,13 @@
         <v>17</v>
       </c>
       <c r="Q32" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R32" s="24" t="s">
         <v>89</v>
       </c>
       <c r="S32" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T32" s="22" t="s">
         <v>83</v>
@@ -3385,7 +3378,7 @@
     </row>
     <row r="33" spans="1:20" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="25" t="s">
@@ -3402,7 +3395,7 @@
         <v>77</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="9" t="s">
@@ -3439,11 +3432,11 @@
     </row>
     <row r="34" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D34" s="27"/>
       <c r="E34" s="9">
@@ -3456,7 +3449,7 @@
         <v>77</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="9" t="s">
@@ -3493,11 +3486,11 @@
     </row>
     <row r="35" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9">
@@ -3510,17 +3503,17 @@
         <v>77</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K35" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="L35" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="L35" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="M35" s="9" t="s">
         <v>18</v>
@@ -3535,7 +3528,7 @@
         <v>17</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R35" s="24" t="s">
         <v>135</v>
@@ -3547,11 +3540,11 @@
     </row>
     <row r="36" spans="1:20" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9">
@@ -3564,7 +3557,7 @@
         <v>77</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="9" t="s">
@@ -3574,7 +3567,7 @@
         <v>17</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M36" s="9" t="s">
         <v>18</v>
@@ -3783,13 +3776,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>3</v>
@@ -3798,7 +3791,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>5</v>
@@ -3807,7 +3800,7 @@
         <v>6</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>7</v>
@@ -3822,13 +3815,13 @@
         <v>10</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="S1" s="7" t="s">
         <v>11</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="U1" s="5"/>
     </row>
@@ -3884,7 +3877,7 @@
         <v>65</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
caricoos gcoos glos nanoos secoora inventories complete
</commit_message>
<xml_diff>
--- a/2024/data/processed/CARICOOS.xlsx
+++ b/2024/data/processed/CARICOOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathew.Biddle\Documents\GitProjects\ioos-asset-inventory\2024\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F784BD58-6FD2-4F45-968A-A06D555886D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F4026A-1B60-45DB-8EA7-8B6CE6EF9C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="195">
   <si>
     <t>Station ID</t>
   </si>
@@ -218,9 +218,6 @@
     <t>05/2021 - present</t>
   </si>
   <si>
-    <t>NREL/CARICOOS</t>
-  </si>
-  <si>
     <t>CARICOOS/CDIP/NREL</t>
   </si>
   <si>
@@ -251,9 +248,6 @@
     <t>2009 - present</t>
   </si>
   <si>
-    <t>CARICOOS, OAP</t>
-  </si>
-  <si>
     <t>PMEL/CARICOOS</t>
   </si>
   <si>
@@ -522,9 +516,6 @@
   </si>
   <si>
     <t>2019-present</t>
-  </si>
-  <si>
-    <t>CARICOOS/OCOVI</t>
   </si>
   <si>
     <t>Weatherflow /CARICOOS/OCOVI</t>
@@ -1528,13 +1519,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U90"/>
+  <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
@@ -1558,7 +1549,7 @@
     <col min="22" max="16384" width="15.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1569,13 +1560,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>3</v>
@@ -1584,19 +1575,19 @@
         <v>4</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>7</v>
@@ -1611,17 +1602,17 @@
         <v>10</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="U1" s="5"/>
     </row>
-    <row r="2" spans="1:21" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
@@ -1674,10 +1665,10 @@
       </c>
       <c r="S2" s="12"/>
       <c r="T2" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
@@ -1730,10 +1721,10 @@
       </c>
       <c r="S3" s="12"/>
       <c r="T3" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>29</v>
       </c>
@@ -1786,10 +1777,10 @@
       </c>
       <c r="S4" s="12"/>
       <c r="T4" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>33</v>
       </c>
@@ -1842,10 +1833,10 @@
       </c>
       <c r="S5" s="12"/>
       <c r="T5" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>37</v>
       </c>
@@ -1900,10 +1891,10 @@
         <v>42</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>43</v>
       </c>
@@ -1958,10 +1949,10 @@
         <v>47</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="6" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>48</v>
       </c>
@@ -2014,10 +2005,10 @@
       </c>
       <c r="S8" s="12"/>
       <c r="T8" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" s="6" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>56</v>
       </c>
@@ -2045,10 +2036,10 @@
         <v>40</v>
       </c>
       <c r="K9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="M9" s="9" t="s">
         <v>18</v>
@@ -2057,7 +2048,7 @@
         <v>53</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>17</v>
@@ -2070,21 +2061,21 @@
       </c>
       <c r="S9" s="12"/>
       <c r="T9" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>68</v>
-      </c>
       <c r="D10" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="15">
         <f>57.22/60 +17</f>
@@ -2097,23 +2088,23 @@
         <v>14</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="15"/>
       <c r="J10" s="15" t="s">
         <v>16</v>
       </c>
       <c r="K10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="N10" s="15" t="s">
         <v>71</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="N10" s="15" t="s">
-        <v>73</v>
       </c>
       <c r="O10" s="15" t="s">
         <v>20</v>
@@ -2122,25 +2113,25 @@
         <v>17</v>
       </c>
       <c r="Q10" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S10" s="18"/>
       <c r="T10" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="9">
@@ -2150,10 +2141,10 @@
         <v>-67.251400000000004</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9" t="s">
@@ -2169,36 +2160,36 @@
         <v>18</v>
       </c>
       <c r="N11" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q11" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="R11" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="P11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q11" s="10" t="s">
+      <c r="S11" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="T11" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="R11" s="11" t="s">
+    </row>
+    <row r="12" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="S11" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="T11" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="9">
@@ -2208,10 +2199,10 @@
         <v>-67.044200000000004</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9" t="s">
@@ -2227,36 +2218,36 @@
         <v>52</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q12" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="S12" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="R12" s="11" t="s">
+      <c r="T12" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="S12" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="T12" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="9">
@@ -2266,10 +2257,10 @@
         <v>-67.044200000000004</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9" t="s">
@@ -2285,36 +2276,36 @@
         <v>18</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="S13" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="T13" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="R13" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="S13" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="T13" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="9">
@@ -2324,10 +2315,10 @@
         <v>-66.617699999999999</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9" t="s">
@@ -2343,36 +2334,36 @@
         <v>18</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="R14" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="P14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q14" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="R14" s="11" t="s">
-        <v>82</v>
-      </c>
       <c r="S14" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="T14" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="9">
@@ -2382,10 +2373,10 @@
         <v>-67.191999999999993</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9" t="s">
@@ -2401,36 +2392,36 @@
         <v>18</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R15" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="S15" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="T15" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="S15" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="T15" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" s="6" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="9">
@@ -2440,10 +2431,10 @@
         <v>-67.261300000000006</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9" t="s">
@@ -2459,34 +2450,34 @@
         <v>18</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="S16" s="12"/>
       <c r="T16" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>108</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21">
@@ -2496,10 +2487,10 @@
         <v>-67.156630000000007</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9" t="s">
@@ -2509,7 +2500,7 @@
         <v>17</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M17" s="9" t="s">
         <v>18</v>
@@ -2518,31 +2509,31 @@
         <v>17</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S17" s="12"/>
       <c r="T17" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="9">
@@ -2552,10 +2543,10 @@
         <v>-64.926400000000001</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="9" t="s">
@@ -2565,7 +2556,7 @@
         <v>17</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M18" s="9" t="s">
         <v>52</v>
@@ -2574,31 +2565,31 @@
         <v>17</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S18" s="12"/>
       <c r="T18" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="21">
@@ -2608,10 +2599,10 @@
         <v>-64.817300000000003</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="9" t="s">
@@ -2621,7 +2612,7 @@
         <v>17</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M19" s="9" t="s">
         <v>18</v>
@@ -2630,31 +2621,31 @@
         <v>17</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S19" s="12"/>
       <c r="T19" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>120</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21">
@@ -2664,10 +2655,10 @@
         <v>-64.892600000000002</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="9" t="s">
@@ -2677,7 +2668,7 @@
         <v>17</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M20" s="9" t="s">
         <v>18</v>
@@ -2686,31 +2677,31 @@
         <v>17</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S20" s="12"/>
       <c r="T20" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21">
@@ -2720,10 +2711,10 @@
         <v>-67.188869999999994</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I21" s="9"/>
       <c r="J21" s="9" t="s">
@@ -2733,7 +2724,7 @@
         <v>17</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M21" s="9" t="s">
         <v>18</v>
@@ -2742,31 +2733,31 @@
         <v>17</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P21" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S21" s="12"/>
       <c r="T21" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21">
@@ -2776,10 +2767,10 @@
         <v>-64.899889999999999</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="9" t="s">
@@ -2789,7 +2780,7 @@
         <v>17</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M22" s="9" t="s">
         <v>18</v>
@@ -2798,31 +2789,31 @@
         <v>17</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P22" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S22" s="12"/>
       <c r="T22" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21">
@@ -2832,10 +2823,10 @@
         <v>-65.227419999999995</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9" t="s">
@@ -2845,7 +2836,7 @@
         <v>17</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M23" s="9" t="s">
         <v>18</v>
@@ -2854,31 +2845,31 @@
         <v>17</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P23" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S23" s="12"/>
       <c r="T23" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>132</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>134</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="21">
@@ -2888,10 +2879,10 @@
         <v>-65.991669999999999</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="9" t="s">
@@ -2901,7 +2892,7 @@
         <v>17</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M24" s="9" t="s">
         <v>18</v>
@@ -2910,31 +2901,31 @@
         <v>17</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="S24" s="12"/>
       <c r="T24" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>138</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21">
@@ -2944,10 +2935,10 @@
         <v>-66.128460000000004</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9" t="s">
@@ -2957,7 +2948,7 @@
         <v>17</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M25" s="9" t="s">
         <v>18</v>
@@ -2966,31 +2957,31 @@
         <v>17</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P25" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R25" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S25" s="12"/>
       <c r="T25" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>141</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21">
@@ -3000,10 +2991,10 @@
         <v>-66.159700000000001</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="9" t="s">
@@ -3013,7 +3004,7 @@
         <v>17</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M26" s="9" t="s">
         <v>18</v>
@@ -3022,31 +3013,31 @@
         <v>17</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P26" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R26" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S26" s="12"/>
       <c r="T26" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>142</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21">
@@ -3056,10 +3047,10 @@
         <v>-65.632000000000005</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="9" t="s">
@@ -3069,7 +3060,7 @@
         <v>17</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M27" s="9" t="s">
         <v>18</v>
@@ -3078,31 +3069,31 @@
         <v>17</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R27" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="S27" s="12"/>
       <c r="T27" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21">
@@ -3112,10 +3103,10 @@
         <v>-64.926609999999997</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9" t="s">
@@ -3125,7 +3116,7 @@
         <v>17</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M28" s="9" t="s">
         <v>18</v>
@@ -3134,31 +3125,31 @@
         <v>17</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P28" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R28" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S28" s="12"/>
       <c r="T28" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>148</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="21">
@@ -3168,10 +3159,10 @@
         <v>-65.082999999999998</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="9" t="s">
@@ -3181,7 +3172,7 @@
         <v>17</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M29" s="9" t="s">
         <v>52</v>
@@ -3190,33 +3181,33 @@
         <v>17</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P29" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R29" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S29" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="T29" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="T29" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>155</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="21">
@@ -3226,10 +3217,10 @@
         <v>-64.966930000000005</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9" t="s">
@@ -3239,7 +3230,7 @@
         <v>17</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M30" s="9" t="s">
         <v>18</v>
@@ -3248,33 +3239,33 @@
         <v>17</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P30" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q30" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S30" s="29" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="T30" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>158</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="21">
@@ -3284,10 +3275,10 @@
         <v>-65.828090000000003</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="9" t="s">
@@ -3297,7 +3288,7 @@
         <v>17</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M31" s="9" t="s">
         <v>18</v>
@@ -3306,27 +3297,27 @@
         <v>17</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P31" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q31" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R31" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="S31" s="12"/>
       <c r="T31" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22">
@@ -3336,20 +3327,20 @@
         <v>-64.95</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I32" s="22"/>
       <c r="J32" s="22" t="s">
         <v>45</v>
       </c>
       <c r="K32" s="22" t="s">
-        <v>161</v>
+        <v>17</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="M32" s="23" t="s">
         <v>18</v>
@@ -3358,31 +3349,31 @@
         <v>17</v>
       </c>
       <c r="O32" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P32" s="23" t="s">
         <v>17</v>
       </c>
       <c r="Q32" s="22" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="R32" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S32" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T32" s="22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="25">
@@ -3392,10 +3383,10 @@
         <v>-67.043800000000005</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="9" t="s">
@@ -3405,7 +3396,7 @@
         <v>17</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M33" s="9" t="s">
         <v>18</v>
@@ -3414,29 +3405,29 @@
         <v>17</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P33" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q33" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R33" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="S33" s="26"/>
       <c r="T33" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D34" s="27"/>
       <c r="E34" s="9">
@@ -3446,10 +3437,10 @@
         <v>-67.191900000000004</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="9" t="s">
@@ -3459,7 +3450,7 @@
         <v>17</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M34" s="9" t="s">
         <v>18</v>
@@ -3468,29 +3459,29 @@
         <v>17</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P34" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R34" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S34" s="26"/>
       <c r="T34" s="22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9">
@@ -3500,20 +3491,20 @@
         <v>-64.956670000000003</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>161</v>
+        <v>17</v>
       </c>
       <c r="L35" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="M35" s="9" t="s">
         <v>18</v>
@@ -3522,29 +3513,29 @@
         <v>17</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P35" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="R35" s="24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="S35" s="26"/>
       <c r="T35" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" s="28" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9">
@@ -3554,10 +3545,10 @@
         <v>-66.98</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="9" t="s">
@@ -3567,7 +3558,7 @@
         <v>17</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="M36" s="9" t="s">
         <v>18</v>
@@ -3576,122 +3567,122 @@
         <v>17</v>
       </c>
       <c r="O36" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P36" s="9" t="s">
         <v>17</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="S36" s="12"/>
       <c r="T36" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q53" s="1"/>
     </row>
-    <row r="54" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q54" s="1"/>
     </row>
-    <row r="55" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q55" s="1"/>
     </row>
-    <row r="56" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q56" s="1"/>
     </row>
-    <row r="57" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q57" s="1"/>
     </row>
-    <row r="58" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q58" s="1"/>
     </row>
-    <row r="59" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q59" s="1"/>
     </row>
-    <row r="60" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q60" s="1"/>
     </row>
-    <row r="61" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q61" s="1"/>
     </row>
-    <row r="62" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q63" s="1"/>
     </row>
-    <row r="64" spans="17:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="17:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q64" s="1"/>
     </row>
-    <row r="65" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -3713,42 +3704,26 @@
       <c r="S70" s="4"/>
       <c r="T70" s="4"/>
     </row>
-    <row r="71" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="Q74" s="1"/>
     </row>
-    <row r="75" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="Q75" s="1"/>
     </row>
-    <row r="76" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.3" right="0.25" top="0.57013888888888897" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3776,13 +3751,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>3</v>
@@ -3791,7 +3766,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>5</v>
@@ -3800,7 +3775,7 @@
         <v>6</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>7</v>
@@ -3815,36 +3790,36 @@
         <v>10</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="S1" s="7" t="s">
         <v>11</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="U1" s="5"/>
     </row>
     <row r="2" spans="2:21" s="6" customFormat="1" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>40</v>
@@ -3874,10 +3849,10 @@
         <v>55</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>